<commit_message>
fix sorting in export
</commit_message>
<xml_diff>
--- a/CVF Report.xlsx
+++ b/CVF Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>CVF REPORT</t>
   </si>
@@ -36,15 +36,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>2019-11-07</t>
-  </si>
-  <si>
-    <t>CV2019-00103</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
   </si>
 </sst>
 </file>
@@ -112,11 +103,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
@@ -424,7 +412,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="F2" sqref="F2"/>
@@ -436,50 +424,36 @@
     <col min="2" max="2" width="7.426758" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="5.570068" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="6.427002" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="6.427002" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add amount in print and export, add amount and description export
</commit_message>
<xml_diff>
--- a/CVF Report.xlsx
+++ b/CVF Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>CVF REPORT</t>
   </si>
@@ -32,10 +32,100 @@
     <t>Bank</t>
   </si>
   <si>
+    <t>Amount</t>
+  </si>
+  <si>
     <t>CV No.</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>2019-10-14</t>
+  </si>
+  <si>
+    <t>11th Street Bed &amp; Breakfast</t>
+  </si>
+  <si>
+    <t>CIB  AUB C/A 204010001065</t>
+  </si>
+  <si>
+    <t>CV2019-00101</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>2019-11-07</t>
+  </si>
+  <si>
+    <t>CV2019-00102</t>
+  </si>
+  <si>
+    <t>CV2019-00106</t>
+  </si>
+  <si>
+    <t>adssdfa</t>
+  </si>
+  <si>
+    <t>CIB CENPRI BDO 006818002580</t>
+  </si>
+  <si>
+    <t>CV2019-00107</t>
+  </si>
+  <si>
+    <t>2019-11-14</t>
+  </si>
+  <si>
+    <t>2GO Express, Inc.</t>
+  </si>
+  <si>
+    <t>CIB ENERGREEN RWMHEEF(DG1-3NEW)</t>
+  </si>
+  <si>
+    <t>CV2019-00108</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>AA Electrical Supply</t>
+  </si>
+  <si>
+    <t>CV2019-00109</t>
+  </si>
+  <si>
+    <t>sdfdaff</t>
+  </si>
+  <si>
+    <t>CV2019-00110</t>
+  </si>
+  <si>
+    <t>CIB CENPRI DLF DG 4-5 (new)</t>
+  </si>
+  <si>
+    <t>CV2019-00111</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>2019-11-13</t>
+  </si>
+  <si>
+    <t>CIB ENERGREEN DLF (DG 1-3 NEW)</t>
+  </si>
+  <si>
+    <t>CV2019-00112</t>
+  </si>
+  <si>
+    <t>sadsdafsad</t>
   </si>
 </sst>
 </file>
@@ -103,9 +193,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -412,48 +508,268 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="7.426758" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.570068" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="6.427002" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="6.427002" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="37.705078" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="6.998291" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>